<commit_message>
Added TCP data table below
</commit_message>
<xml_diff>
--- a/docs/Closed_DG_Stores_27_May.xlsx
+++ b/docs/Closed_DG_Stores_27_May.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidfit\OneDrive - Cisco\Documents\Cisco\Comcast-Escalation\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidfit\OneDrive - Cisco\Documents\Programming\RegistrationAnalysisTool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3088899E-E04C-4D96-8B20-3482537C1DCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E0933-5907-4953-A6D6-400FE26A8580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="3345" windowWidth="19200" windowHeight="8520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed shops" sheetId="1" r:id="rId1"/>
     <sheet name="nuregisteredshops" sheetId="2" r:id="rId2"/>
     <sheet name="unregistered open shops" sheetId="3" r:id="rId3"/>
+    <sheet name="tcp shops" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17792" uniqueCount="1338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17830" uniqueCount="1374">
   <si>
     <t>DGC#00068</t>
   </si>
@@ -4036,13 +4037,121 @@
   </si>
   <si>
     <t>DGC#10491</t>
+  </si>
+  <si>
+    <t>DGC#00152</t>
+  </si>
+  <si>
+    <t>DGC#01280</t>
+  </si>
+  <si>
+    <t>DGC#01453</t>
+  </si>
+  <si>
+    <t>DGC#01531</t>
+  </si>
+  <si>
+    <t>DGC#01904</t>
+  </si>
+  <si>
+    <t>DGC#01965</t>
+  </si>
+  <si>
+    <t>DGC#03724</t>
+  </si>
+  <si>
+    <t>DGC#04259</t>
+  </si>
+  <si>
+    <t>DGC#04438</t>
+  </si>
+  <si>
+    <t>DGC#04701</t>
+  </si>
+  <si>
+    <t>DGC#05816</t>
+  </si>
+  <si>
+    <t>DGC#07803</t>
+  </si>
+  <si>
+    <t>DGC#07812</t>
+  </si>
+  <si>
+    <t>DGC#08917</t>
+  </si>
+  <si>
+    <t>DGC#09481</t>
+  </si>
+  <si>
+    <t>DGC#09934</t>
+  </si>
+  <si>
+    <t>DGC#12386</t>
+  </si>
+  <si>
+    <t>DGC#14864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGC#17276	</t>
+  </si>
+  <si>
+    <t>DGC#17596</t>
+  </si>
+  <si>
+    <t>DGC#17677</t>
+  </si>
+  <si>
+    <t>DGC#17687</t>
+  </si>
+  <si>
+    <t>DGC#17767</t>
+  </si>
+  <si>
+    <t>DGC#17783</t>
+  </si>
+  <si>
+    <t>DGC#17822</t>
+  </si>
+  <si>
+    <t>DGC#17829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGC#17833	</t>
+  </si>
+  <si>
+    <t>DGC#17911</t>
+  </si>
+  <si>
+    <t>DGC#18216</t>
+  </si>
+  <si>
+    <t>DGC#18320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGC#18844	</t>
+  </si>
+  <si>
+    <t>DGC#18858</t>
+  </si>
+  <si>
+    <t>DGC#19004</t>
+  </si>
+  <si>
+    <t>DGC#19076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGC#19119	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGC#19206	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4056,19 +4165,57 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC1C7D0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC1C7D0"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFC1C7D0"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC1C7D0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC1C7D0"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC1C7D0"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -4077,13 +4224,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4401,7 +4555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A93"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
@@ -36058,7 +36212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+    <sheetView topLeftCell="A234" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -60957,4 +61111,214 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37631153-6DDB-49D8-9559-BBA7E98F4B5D}">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add total to view
</commit_message>
<xml_diff>
--- a/docs/Closed_DG_Stores_27_May.xlsx
+++ b/docs/Closed_DG_Stores_27_May.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidfit\OneDrive - Cisco\Documents\Programming\RegistrationAnalysisTool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E0933-5907-4953-A6D6-400FE26A8580}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ED7B15-2B64-4B08-AE36-E0806F44AACA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="3345" windowWidth="19200" windowHeight="8520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3240" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="closed shops" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17830" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17831" uniqueCount="1375">
   <si>
     <t>DGC#00068</t>
   </si>
@@ -4145,6 +4145,9 @@
   </si>
   <si>
     <t xml:space="preserve">DGC#19206	</t>
+  </si>
+  <si>
+    <t>Name1</t>
   </si>
 </sst>
 </file>
@@ -61115,10 +61118,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37631153-6DDB-49D8-9559-BBA7E98F4B5D}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -61127,193 +61130,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1338</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>1339</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>318</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>1344</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B18" s="4"/>
+        <v>1353</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>1355</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>1356</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>201</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>1362</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>1363</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>1364</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>1367</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>1368</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
         <v>1371</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>1373</v>
       </c>
     </row>

</xml_diff>